<commit_message>
got part 1 working started pt 2
</commit_message>
<xml_diff>
--- a/ClueGame/ClueBoardLayout.xlsx
+++ b/ClueGame/ClueBoardLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hornet\Users\s\sbride\adit\My Documents\CSCI306\C12A-2 Clue Layout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\CSCI306\C12A-2 Clue Layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="38">
   <si>
     <t>B</t>
   </si>
@@ -126,13 +126,25 @@
   </si>
   <si>
     <t>Door</t>
+  </si>
+  <si>
+    <t>Adjancency Lists inside rooms</t>
+  </si>
+  <si>
+    <t>Room Entrances</t>
+  </si>
+  <si>
+    <t>Room Exits</t>
+  </si>
+  <si>
+    <t>Targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +159,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF66CCFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +252,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -240,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,6 +352,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -307,6 +389,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66CCFF"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FF9966FF"/>
       <color rgb="FF66FF33"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FFFF00FF"/>
@@ -588,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +689,7 @@
       <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="28" t="s">
         <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -625,7 +710,7 @@
       <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="27" t="s">
         <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
@@ -651,7 +736,7 @@
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -660,10 +745,10 @@
       <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -695,10 +780,10 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -707,16 +792,16 @@
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="20" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -760,16 +845,16 @@
       <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="22" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="18" t="s">
+      <c r="J4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -816,7 +901,7 @@
       <c r="J5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -825,7 +910,7 @@
       <c r="M5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="27" t="s">
         <v>21</v>
       </c>
       <c r="O5" s="6">
@@ -913,10 +998,10 @@
       <c r="K7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="18" t="s">
+      <c r="L7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>8</v>
       </c>
       <c r="N7" s="7" t="s">
@@ -1060,7 +1145,7 @@
       <c r="M10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N10" s="25" t="s">
         <v>21</v>
       </c>
       <c r="O10" s="6">
@@ -1068,7 +1153,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1259,7 +1344,7 @@
       <c r="A15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1309,10 +1394,10 @@
       <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1377,7 +1462,7 @@
       <c r="I17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" s="22" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -1418,13 +1503,13 @@
       <c r="G18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="20" t="s">
         <v>18</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="J18" s="21" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -1456,13 +1541,13 @@
       <c r="D19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="25" t="s">
         <v>21</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="24" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="18" t="s">
@@ -1494,7 +1579,7 @@
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1538,7 +1623,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1632,7 +1717,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -1650,7 +1735,7 @@
       <c r="F23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="27" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="12" t="s">
@@ -1662,7 +1747,7 @@
       <c r="J23" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L23" s="2" t="s">
@@ -1727,29 +1812,50 @@
       <c r="B28" s="17" t="s">
         <v>22</v>
       </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="17" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="17" t="s">
         <v>23</v>
       </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="17" t="s">
         <v>26</v>
+      </c>
+      <c r="D32" s="27"/>
+      <c r="E32" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>